<commit_message>
general models update; 2 models added
</commit_message>
<xml_diff>
--- a/Models/ABNB.xlsx
+++ b/Models/ABNB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/36a87f973740ffce/Documents/Personal/Finance/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1675" documentId="8_{01B29E05-4074-C24F-9F5A-60F75487FDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F886CBE-C049-4E38-BEA6-7E508607BF9B}"/>
+  <xr:revisionPtr revIDLastSave="1681" documentId="8_{01B29E05-4074-C24F-9F5A-60F75487FDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63EE0E82-45C2-9646-9A3A-894EDF08B72C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E36FCDD1-B29B-B64E-8BC8-95300EC8866E}"/>
+    <workbookView xWindow="-120" yWindow="680" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E36FCDD1-B29B-B64E-8BC8-95300EC8866E}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1078,10 +1078,10 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" s="5" customFormat="1">
@@ -1212,7 +1212,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="2:11">
+    <row r="16" spans="2:11" ht="14">
       <c r="B16" t="s">
         <v>15</v>
       </c>
@@ -1557,25 +1557,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC8C7F3-F2C1-7648-A25C-50F3C2F80138}">
   <dimension ref="A1:VG53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="AQ21" sqref="AQ21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="10.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="2" customWidth="1"/>
-    <col min="7" max="14" width="10.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="2" customWidth="1"/>
-    <col min="17" max="22" width="10.85546875" style="2"/>
-    <col min="23" max="24" width="10.85546875" style="21"/>
-    <col min="25" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="1" width="4.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="2" customWidth="1"/>
+    <col min="7" max="14" width="10.33203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="2" customWidth="1"/>
+    <col min="17" max="22" width="10.83203125" style="2"/>
+    <col min="23" max="24" width="10.83203125" style="21"/>
+    <col min="25" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -3480,27 +3480,27 @@
         <v>2648</v>
       </c>
       <c r="AF19" s="8">
-        <f>AF6*$AE$38</f>
+        <f t="shared" ref="AF19:AK19" si="28">AF6*$AE$38</f>
         <v>3045.2</v>
       </c>
       <c r="AG19" s="8">
-        <f>AG6*$AE$38</f>
+        <f t="shared" si="28"/>
         <v>3501.9799999999996</v>
       </c>
       <c r="AH19" s="8">
-        <f>AH6*$AE$38</f>
+        <f t="shared" si="28"/>
         <v>4027.2769999999996</v>
       </c>
       <c r="AI19" s="8">
-        <f>AI6*$AE$38</f>
+        <f t="shared" si="28"/>
         <v>4631.3685499999992</v>
       </c>
       <c r="AJ19" s="8">
-        <f>AJ6*$AE$38</f>
+        <f t="shared" si="28"/>
         <v>5326.0738324999984</v>
       </c>
       <c r="AK19" s="8">
-        <f>AK6*$AE$38</f>
+        <f t="shared" si="28"/>
         <v>6124.9849073749974</v>
       </c>
       <c r="AM19" s="8" t="s">
@@ -3611,79 +3611,79 @@
         <v>3.8251801591547467E-3</v>
       </c>
       <c r="E22" s="17">
-        <f t="shared" ref="E22:W22" si="28">(E21-D21)/E21</f>
+        <f t="shared" ref="E22:W22" si="29">(E21-D21)/E21</f>
         <v>0.11927902515323897</v>
       </c>
       <c r="F22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.13463001258116289</v>
       </c>
       <c r="G22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.42466220713525032</v>
       </c>
       <c r="H22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>1.7620259620524433E-2</v>
       </c>
       <c r="I22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.10291150229647056</v>
       </c>
       <c r="J22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.4980261302755423E-3</v>
       </c>
       <c r="K22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-7.2277165354330639E-2</v>
       </c>
       <c r="L22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>7.1637426900584791E-2</v>
       </c>
       <c r="M22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.4641288433382138E-3</v>
       </c>
       <c r="N22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-4.4117647058823529E-3</v>
       </c>
       <c r="O22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.4925373134328358E-2</v>
       </c>
       <c r="P22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-7.5187969924812026E-3</v>
       </c>
       <c r="Q22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-7.575757575757576E-3</v>
       </c>
       <c r="R22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>3.0211480362537764E-3</v>
       </c>
       <c r="S22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.2232415902140673E-2</v>
       </c>
       <c r="T22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-7.7041602465331279E-3</v>
       </c>
       <c r="U22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-1.0903426791277258E-2</v>
       </c>
       <c r="V22" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>4.6511627906976744E-3</v>
       </c>
       <c r="W22" s="25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>-2.0569620253164556E-2</v>
       </c>
       <c r="X22" s="25">
@@ -3855,15 +3855,15 @@
         <v>23</v>
       </c>
       <c r="AA25" s="2">
-        <f t="shared" ref="AA25:AA26" si="29">SUM(C25:F25)</f>
+        <f t="shared" ref="AA25:AA26" si="30">SUM(C25:F25)</f>
         <v>37.4</v>
       </c>
       <c r="AB25" s="2">
-        <f t="shared" ref="AB25:AB26" si="30">SUM(G25:J25)</f>
+        <f t="shared" ref="AB25:AB26" si="31">SUM(G25:J25)</f>
         <v>25.299999999999997</v>
       </c>
       <c r="AC25" s="2">
-        <f t="shared" ref="AC25:AC26" si="31">SUM(K25:N25)</f>
+        <f t="shared" ref="AC25:AC26" si="32">SUM(K25:N25)</f>
         <v>25</v>
       </c>
       <c r="AD25" s="2">
@@ -3884,99 +3884,99 @@
         <v>-578.6</v>
       </c>
       <c r="D26" s="8">
-        <f t="shared" ref="D26:N26" si="32">D24-D25</f>
+        <f t="shared" ref="D26:N26" si="33">D24-D25</f>
         <v>-263.09999999999997</v>
       </c>
       <c r="E26" s="8">
+        <f t="shared" si="33"/>
+        <v>330.7</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="33"/>
+        <v>-272.5</v>
+      </c>
+      <c r="G26" s="8">
+        <f t="shared" si="33"/>
+        <v>610.29999999999995</v>
+      </c>
+      <c r="H26" s="8">
+        <f t="shared" si="33"/>
+        <v>782.4</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" si="33"/>
+        <v>522.19999999999993</v>
+      </c>
+      <c r="J26" s="8">
+        <f t="shared" si="33"/>
+        <v>377.6</v>
+      </c>
+      <c r="K26" s="8">
+        <f t="shared" si="33"/>
+        <v>1196</v>
+      </c>
+      <c r="L26" s="8">
+        <f t="shared" si="33"/>
+        <v>795</v>
+      </c>
+      <c r="M26" s="8">
+        <f t="shared" si="33"/>
+        <v>959</v>
+      </c>
+      <c r="N26" s="8">
+        <f t="shared" si="33"/>
+        <v>455</v>
+      </c>
+      <c r="O26" s="8">
+        <f t="shared" ref="O26:W26" si="34">O24-O25</f>
+        <v>1581</v>
+      </c>
+      <c r="P26" s="8">
+        <f t="shared" si="34"/>
+        <v>900</v>
+      </c>
+      <c r="Q26" s="8">
+        <f t="shared" si="34"/>
+        <v>1310</v>
+      </c>
+      <c r="R26" s="8">
+        <f t="shared" si="34"/>
+        <v>46</v>
+      </c>
+      <c r="S26" s="8">
+        <f t="shared" si="34"/>
+        <v>1909</v>
+      </c>
+      <c r="T26" s="8">
+        <f t="shared" si="34"/>
+        <v>1043</v>
+      </c>
+      <c r="U26" s="8">
+        <f t="shared" si="34"/>
+        <v>1074</v>
+      </c>
+      <c r="V26" s="8">
+        <f t="shared" si="34"/>
+        <v>458</v>
+      </c>
+      <c r="W26" s="24">
+        <f t="shared" si="34"/>
+        <v>1781</v>
+      </c>
+      <c r="X26" s="24">
+        <f t="shared" ref="X26" si="35">X24-X25</f>
+        <v>952</v>
+      </c>
+      <c r="AA26" s="8">
+        <f t="shared" si="30"/>
+        <v>-783.5</v>
+      </c>
+      <c r="AB26" s="8">
+        <f t="shared" si="31"/>
+        <v>2292.4999999999995</v>
+      </c>
+      <c r="AC26" s="8">
         <f t="shared" si="32"/>
-        <v>330.7</v>
-      </c>
-      <c r="F26" s="8">
-        <f t="shared" si="32"/>
-        <v>-272.5</v>
-      </c>
-      <c r="G26" s="8">
-        <f t="shared" si="32"/>
-        <v>610.29999999999995</v>
-      </c>
-      <c r="H26" s="8">
-        <f t="shared" si="32"/>
-        <v>782.4</v>
-      </c>
-      <c r="I26" s="8">
-        <f t="shared" si="32"/>
-        <v>522.19999999999993</v>
-      </c>
-      <c r="J26" s="8">
-        <f t="shared" si="32"/>
-        <v>377.6</v>
-      </c>
-      <c r="K26" s="8">
-        <f t="shared" si="32"/>
-        <v>1196</v>
-      </c>
-      <c r="L26" s="8">
-        <f t="shared" si="32"/>
-        <v>795</v>
-      </c>
-      <c r="M26" s="8">
-        <f t="shared" si="32"/>
-        <v>959</v>
-      </c>
-      <c r="N26" s="8">
-        <f t="shared" si="32"/>
-        <v>455</v>
-      </c>
-      <c r="O26" s="8">
-        <f t="shared" ref="O26:W26" si="33">O24-O25</f>
-        <v>1581</v>
-      </c>
-      <c r="P26" s="8">
-        <f t="shared" si="33"/>
-        <v>900</v>
-      </c>
-      <c r="Q26" s="8">
-        <f t="shared" si="33"/>
-        <v>1310</v>
-      </c>
-      <c r="R26" s="8">
-        <f t="shared" si="33"/>
-        <v>46</v>
-      </c>
-      <c r="S26" s="8">
-        <f t="shared" si="33"/>
-        <v>1909</v>
-      </c>
-      <c r="T26" s="8">
-        <f t="shared" si="33"/>
-        <v>1043</v>
-      </c>
-      <c r="U26" s="8">
-        <f t="shared" si="33"/>
-        <v>1074</v>
-      </c>
-      <c r="V26" s="8">
-        <f t="shared" si="33"/>
-        <v>458</v>
-      </c>
-      <c r="W26" s="24">
-        <f t="shared" si="33"/>
-        <v>1781</v>
-      </c>
-      <c r="X26" s="24">
-        <f t="shared" ref="X26" si="34">X24-X25</f>
-        <v>952</v>
-      </c>
-      <c r="AA26" s="8">
-        <f t="shared" si="29"/>
-        <v>-783.5</v>
-      </c>
-      <c r="AB26" s="8">
-        <f t="shared" si="30"/>
-        <v>2292.4999999999995</v>
-      </c>
-      <c r="AC26" s="8">
-        <f t="shared" si="31"/>
         <v>3405</v>
       </c>
       <c r="AD26" s="8">
@@ -3992,2191 +3992,2191 @@
         <v>5156.5999999999995</v>
       </c>
       <c r="AG26" s="8">
-        <f t="shared" ref="AG26:AK26" si="35">AF26*1.15</f>
+        <f t="shared" ref="AG26:AK26" si="36">AF26*1.15</f>
         <v>5930.0899999999992</v>
       </c>
       <c r="AH26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>6819.6034999999983</v>
       </c>
       <c r="AI26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7842.5440249999974</v>
       </c>
       <c r="AJ26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>9018.9256287499957</v>
       </c>
       <c r="AK26" s="8">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>10371.764473062494</v>
       </c>
       <c r="AL26" s="8">
-        <f t="shared" ref="AL26:CW26" si="36">AK26*(1+$AN$15)</f>
+        <f t="shared" ref="AL26:CW26" si="37">AK26*(1+$AN$15)</f>
         <v>10579.199762523744</v>
       </c>
       <c r="AM26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10790.783757774219</v>
       </c>
       <c r="AN26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11006.599432929705</v>
       </c>
       <c r="AO26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11226.731421588298</v>
       </c>
       <c r="AP26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11451.266050020064</v>
       </c>
       <c r="AQ26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11680.291371020465</v>
       </c>
       <c r="AR26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11913.897198440874</v>
       </c>
       <c r="AS26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>12152.175142409693</v>
       </c>
       <c r="AT26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>12395.218645257886</v>
       </c>
       <c r="AU26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>12643.123018163044</v>
       </c>
       <c r="AV26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>12895.985478526305</v>
       </c>
       <c r="AW26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>13153.905188096831</v>
       </c>
       <c r="AX26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>13416.983291858767</v>
       </c>
       <c r="AY26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>13685.322957695942</v>
       </c>
       <c r="AZ26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>13959.02941684986</v>
       </c>
       <c r="BA26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>14238.210005186858</v>
       </c>
       <c r="BB26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>14522.974205290595</v>
       </c>
       <c r="BC26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>14813.433689396406</v>
       </c>
       <c r="BD26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>15109.702363184335</v>
       </c>
       <c r="BE26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>15411.896410448022</v>
       </c>
       <c r="BF26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>15720.134338656982</v>
       </c>
       <c r="BG26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>16034.537025430122</v>
       </c>
       <c r="BH26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>16355.227765938724</v>
       </c>
       <c r="BI26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>16682.332321257498</v>
       </c>
       <c r="BJ26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>17015.978967682648</v>
       </c>
       <c r="BK26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>17356.298547036302</v>
       </c>
       <c r="BL26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>17703.42451797703</v>
       </c>
       <c r="BM26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>18057.493008336569</v>
       </c>
       <c r="BN26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>18418.642868503299</v>
       </c>
       <c r="BO26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>18787.015725873363</v>
       </c>
       <c r="BP26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>19162.756040390832</v>
       </c>
       <c r="BQ26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>19546.01116119865</v>
       </c>
       <c r="BR26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>19936.931384422624</v>
       </c>
       <c r="BS26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>20335.670012111077</v>
       </c>
       <c r="BT26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>20742.383412353298</v>
       </c>
       <c r="BU26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>21157.231080600362</v>
       </c>
       <c r="BV26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>21580.375702212372</v>
       </c>
       <c r="BW26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>22011.98321625662</v>
       </c>
       <c r="BX26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>22452.222880581754</v>
       </c>
       <c r="BY26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>22901.267338193389</v>
       </c>
       <c r="BZ26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23359.292684957258</v>
       </c>
       <c r="CA26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23826.478538656404</v>
       </c>
       <c r="CB26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>24303.008109429531</v>
       </c>
       <c r="CC26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>24789.068271618122</v>
       </c>
       <c r="CD26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>25284.849637050484</v>
       </c>
       <c r="CE26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>25790.546629791494</v>
       </c>
       <c r="CF26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>26306.357562387326</v>
       </c>
       <c r="CG26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>26832.484713635073</v>
       </c>
       <c r="CH26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>27369.134407907775</v>
       </c>
       <c r="CI26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>27916.517096065931</v>
       </c>
       <c r="CJ26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>28474.84743798725</v>
       </c>
       <c r="CK26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>29044.344386746994</v>
       </c>
       <c r="CL26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>29625.231274481936</v>
       </c>
       <c r="CM26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>30217.735899971576</v>
       </c>
       <c r="CN26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>30822.090617971007</v>
       </c>
       <c r="CO26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>31438.53243033043</v>
       </c>
       <c r="CP26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>32067.303078937039</v>
       </c>
       <c r="CQ26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>32708.649140515779</v>
       </c>
       <c r="CR26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>33362.822123326099</v>
       </c>
       <c r="CS26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>34030.078565792624</v>
       </c>
       <c r="CT26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>34710.68013710848</v>
       </c>
       <c r="CU26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>35404.893739850653</v>
       </c>
       <c r="CV26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>36112.991614647668</v>
       </c>
       <c r="CW26" s="8">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>36835.251446940623</v>
       </c>
       <c r="CX26" s="8">
-        <f t="shared" ref="CX26:FI26" si="37">CW26*(1+$AN$15)</f>
+        <f t="shared" ref="CX26:FI26" si="38">CW26*(1+$AN$15)</f>
         <v>37571.956475879437</v>
       </c>
       <c r="CY26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>38323.395605397025</v>
       </c>
       <c r="CZ26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>39089.863517504964</v>
       </c>
       <c r="DA26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>39871.660787855064</v>
       </c>
       <c r="DB26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>40669.094003612168</v>
       </c>
       <c r="DC26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>41482.475883684412</v>
       </c>
       <c r="DD26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>42312.125401358098</v>
       </c>
       <c r="DE26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>43158.367909385262</v>
       </c>
       <c r="DF26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>44021.535267572966</v>
       </c>
       <c r="DG26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>44901.965972924423</v>
       </c>
       <c r="DH26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>45800.005292382913</v>
       </c>
       <c r="DI26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>46716.005398230569</v>
       </c>
       <c r="DJ26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>47650.325506195179</v>
       </c>
       <c r="DK26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>48603.33201631908</v>
       </c>
       <c r="DL26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>49575.398656645462</v>
       </c>
       <c r="DM26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>50566.906629778372</v>
       </c>
       <c r="DN26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>51578.244762373943</v>
       </c>
       <c r="DO26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>52609.809657621423</v>
       </c>
       <c r="DP26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>53662.00585077385</v>
       </c>
       <c r="DQ26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>54735.245967789328</v>
       </c>
       <c r="DR26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>55829.950887145118</v>
       </c>
       <c r="DS26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>56946.549904888023</v>
       </c>
       <c r="DT26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>58085.480902985786</v>
       </c>
       <c r="DU26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>59247.190521045501</v>
       </c>
       <c r="DV26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>60432.134331466412</v>
       </c>
       <c r="DW26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>61640.777018095738</v>
       </c>
       <c r="DX26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>62873.592558457654</v>
       </c>
       <c r="DY26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>64131.064409626808</v>
       </c>
       <c r="DZ26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>65413.685697819346</v>
       </c>
       <c r="EA26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>66721.959411775737</v>
       </c>
       <c r="EB26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>68056.398600011249</v>
       </c>
       <c r="EC26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>69417.526572011469</v>
       </c>
       <c r="ED26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>70805.877103451698</v>
       </c>
       <c r="EE26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>72221.994645520739</v>
       </c>
       <c r="EF26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>73666.43453843116</v>
       </c>
       <c r="EG26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>75139.763229199787</v>
       </c>
       <c r="EH26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>76642.558493783785</v>
       </c>
       <c r="EI26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>78175.409663659462</v>
       </c>
       <c r="EJ26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>79738.917856932647</v>
       </c>
       <c r="EK26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>81333.6962140713</v>
       </c>
       <c r="EL26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>82960.370138352722</v>
       </c>
       <c r="EM26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>84619.577541119783</v>
       </c>
       <c r="EN26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>86311.969091942185</v>
       </c>
       <c r="EO26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>88038.208473781036</v>
       </c>
       <c r="EP26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>89798.972643256653</v>
       </c>
       <c r="EQ26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>91594.952096121793</v>
       </c>
       <c r="ER26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>93426.851138044236</v>
       </c>
       <c r="ES26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>95295.388160805116</v>
       </c>
       <c r="ET26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>97201.295924021222</v>
       </c>
       <c r="EU26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>99145.321842501653</v>
       </c>
       <c r="EV26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>101128.22827935169</v>
       </c>
       <c r="EW26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>103150.79284493873</v>
       </c>
       <c r="EX26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>105213.80870183751</v>
       </c>
       <c r="EY26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>107318.08487587426</v>
       </c>
       <c r="EZ26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>109464.44657339175</v>
       </c>
       <c r="FA26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>111653.73550485958</v>
       </c>
       <c r="FB26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>113886.81021495677</v>
       </c>
       <c r="FC26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>116164.54641925592</v>
       </c>
       <c r="FD26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>118487.83734764103</v>
       </c>
       <c r="FE26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>120857.59409459386</v>
       </c>
       <c r="FF26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>123274.74597648575</v>
       </c>
       <c r="FG26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>125740.24089601547</v>
       </c>
       <c r="FH26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>128255.04571393579</v>
       </c>
       <c r="FI26" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>130820.14662821451</v>
       </c>
       <c r="FJ26" s="8">
-        <f t="shared" ref="FJ26:HU26" si="38">FI26*(1+$AN$15)</f>
+        <f t="shared" ref="FJ26:HU26" si="39">FI26*(1+$AN$15)</f>
         <v>133436.5495607788</v>
       </c>
       <c r="FK26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>136105.28055199439</v>
       </c>
       <c r="FL26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>138827.38616303427</v>
       </c>
       <c r="FM26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>141603.93388629495</v>
       </c>
       <c r="FN26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>144436.01256402084</v>
       </c>
       <c r="FO26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>147324.73281530125</v>
       </c>
       <c r="FP26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>150271.22747160727</v>
       </c>
       <c r="FQ26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>153276.65202103942</v>
       </c>
       <c r="FR26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>156342.18506146022</v>
       </c>
       <c r="FS26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>159469.02876268941</v>
       </c>
       <c r="FT26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>162658.40933794322</v>
       </c>
       <c r="FU26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>165911.57752470209</v>
       </c>
       <c r="FV26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>169229.80907519613</v>
       </c>
       <c r="FW26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>172614.40525670006</v>
       </c>
       <c r="FX26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>176066.69336183407</v>
       </c>
       <c r="FY26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>179588.02722907075</v>
       </c>
       <c r="FZ26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>183179.78777365218</v>
       </c>
       <c r="GA26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>186843.38352912522</v>
       </c>
       <c r="GB26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>190580.25119970774</v>
       </c>
       <c r="GC26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>194391.85622370191</v>
       </c>
       <c r="GD26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>198279.69334817596</v>
       </c>
       <c r="GE26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>202245.28721513948</v>
       </c>
       <c r="GF26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>206290.19295944227</v>
       </c>
       <c r="GG26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>210415.99681863113</v>
       </c>
       <c r="GH26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>214624.31675500376</v>
       </c>
       <c r="GI26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>218916.80309010384</v>
       </c>
       <c r="GJ26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>223295.13915190593</v>
       </c>
       <c r="GK26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>227761.04193494405</v>
       </c>
       <c r="GL26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>232316.26277364293</v>
       </c>
       <c r="GM26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>236962.58802911578</v>
       </c>
       <c r="GN26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>241701.8397896981</v>
       </c>
       <c r="GO26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>246535.87658549208</v>
       </c>
       <c r="GP26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>251466.59411720192</v>
       </c>
       <c r="GQ26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>256495.92599954596</v>
       </c>
       <c r="GR26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>261625.84451953688</v>
       </c>
       <c r="GS26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>266858.3614099276</v>
       </c>
       <c r="GT26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>272195.52863812615</v>
       </c>
       <c r="GU26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>277639.4392108887</v>
       </c>
       <c r="GV26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>283192.22799510648</v>
       </c>
       <c r="GW26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>288856.07255500864</v>
       </c>
       <c r="GX26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>294633.1940061088</v>
       </c>
       <c r="GY26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>300525.85788623098</v>
       </c>
       <c r="GZ26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>306536.37504395563</v>
       </c>
       <c r="HA26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>312667.10254483472</v>
       </c>
       <c r="HB26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>318920.44459573145</v>
       </c>
       <c r="HC26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>325298.85348764609</v>
       </c>
       <c r="HD26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>331804.83055739902</v>
       </c>
       <c r="HE26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>338440.927168547</v>
       </c>
       <c r="HF26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>345209.74571191793</v>
       </c>
       <c r="HG26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>352113.94062615628</v>
       </c>
       <c r="HH26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>359156.2194386794</v>
       </c>
       <c r="HI26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>366339.34382745298</v>
       </c>
       <c r="HJ26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>373666.13070400205</v>
       </c>
       <c r="HK26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>381139.45331808209</v>
       </c>
       <c r="HL26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>388762.24238444376</v>
       </c>
       <c r="HM26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>396537.48723213264</v>
       </c>
       <c r="HN26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>404468.23697677528</v>
       </c>
       <c r="HO26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>412557.60171631078</v>
       </c>
       <c r="HP26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>420808.753750637</v>
       </c>
       <c r="HQ26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>429224.92882564972</v>
       </c>
       <c r="HR26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>437809.42740216275</v>
       </c>
       <c r="HS26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>446565.615950206</v>
       </c>
       <c r="HT26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>455496.92826921016</v>
       </c>
       <c r="HU26" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>464606.86683459434</v>
       </c>
       <c r="HV26" s="8">
-        <f t="shared" ref="HV26:KG26" si="39">HU26*(1+$AN$15)</f>
+        <f t="shared" ref="HV26:KG26" si="40">HU26*(1+$AN$15)</f>
         <v>473899.00417128624</v>
       </c>
       <c r="HW26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>483376.98425471201</v>
       </c>
       <c r="HX26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>493044.52393980627</v>
       </c>
       <c r="HY26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>502905.41441860242</v>
       </c>
       <c r="HZ26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>512963.52270697447</v>
       </c>
       <c r="IA26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>523222.79316111398</v>
       </c>
       <c r="IB26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>533687.24902433623</v>
       </c>
       <c r="IC26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>544360.99400482292</v>
       </c>
       <c r="ID26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>555248.21388491942</v>
       </c>
       <c r="IE26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>566353.17816261784</v>
       </c>
       <c r="IF26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>577680.24172587018</v>
       </c>
       <c r="IG26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>589233.84656038764</v>
       </c>
       <c r="IH26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>601018.52349159541</v>
       </c>
       <c r="II26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>613038.89396142727</v>
       </c>
       <c r="IJ26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>625299.67184065585</v>
       </c>
       <c r="IK26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>637805.66527746897</v>
       </c>
       <c r="IL26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>650561.77858301834</v>
       </c>
       <c r="IM26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>663573.01415467868</v>
       </c>
       <c r="IN26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>676844.4744377723</v>
       </c>
       <c r="IO26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>690381.36392652779</v>
       </c>
       <c r="IP26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>704188.99120505841</v>
       </c>
       <c r="IQ26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>718272.77102915954</v>
       </c>
       <c r="IR26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>732638.2264497428</v>
       </c>
       <c r="IS26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>747290.99097873771</v>
       </c>
       <c r="IT26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>762236.81079831242</v>
       </c>
       <c r="IU26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>777481.54701427871</v>
       </c>
       <c r="IV26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>793031.17795456434</v>
       </c>
       <c r="IW26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>808891.80151365569</v>
       </c>
       <c r="IX26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>825069.63754392881</v>
       </c>
       <c r="IY26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>841571.03029480739</v>
       </c>
       <c r="IZ26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>858402.45090070355</v>
       </c>
       <c r="JA26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>875570.49991871766</v>
       </c>
       <c r="JB26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>893081.90991709207</v>
       </c>
       <c r="JC26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>910943.54811543389</v>
       </c>
       <c r="JD26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>929162.41907774261</v>
       </c>
       <c r="JE26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>947745.66745929746</v>
       </c>
       <c r="JF26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>966700.58080848341</v>
       </c>
       <c r="JG26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>986034.59242465312</v>
       </c>
       <c r="JH26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1005755.2842731462</v>
       </c>
       <c r="JI26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1025870.3899586091</v>
       </c>
       <c r="JJ26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1046387.7977577813</v>
       </c>
       <c r="JK26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1067315.553712937</v>
       </c>
       <c r="JL26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1088661.8647871958</v>
       </c>
       <c r="JM26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1110435.1020829398</v>
       </c>
       <c r="JN26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1132643.8041245986</v>
       </c>
       <c r="JO26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1155296.6802070907</v>
       </c>
       <c r="JP26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1178402.6138112326</v>
       </c>
       <c r="JQ26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1201970.6660874572</v>
       </c>
       <c r="JR26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1226010.0794092063</v>
       </c>
       <c r="JS26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1250530.2809973904</v>
       </c>
       <c r="JT26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1275540.8866173383</v>
       </c>
       <c r="JU26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1301051.704349685</v>
       </c>
       <c r="JV26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1327072.7384366787</v>
       </c>
       <c r="JW26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1353614.1932054122</v>
       </c>
       <c r="JX26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1380686.4770695206</v>
       </c>
       <c r="JY26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1408300.2066109111</v>
       </c>
       <c r="JZ26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1436466.2107431293</v>
       </c>
       <c r="KA26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1465195.5349579919</v>
       </c>
       <c r="KB26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1494499.4456571518</v>
       </c>
       <c r="KC26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1524389.4345702948</v>
       </c>
       <c r="KD26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1554877.2232617007</v>
       </c>
       <c r="KE26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1585974.7677269347</v>
       </c>
       <c r="KF26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1617694.2630814735</v>
       </c>
       <c r="KG26" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1650048.148343103</v>
       </c>
       <c r="KH26" s="8">
-        <f t="shared" ref="KH26:MS26" si="40">KG26*(1+$AN$15)</f>
+        <f t="shared" ref="KH26:MS26" si="41">KG26*(1+$AN$15)</f>
         <v>1683049.1113099651</v>
       </c>
       <c r="KI26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1716710.0935361644</v>
       </c>
       <c r="KJ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1751044.2954068878</v>
       </c>
       <c r="KK26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1786065.1813150255</v>
       </c>
       <c r="KL26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1821786.4849413261</v>
       </c>
       <c r="KM26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1858222.2146401526</v>
       </c>
       <c r="KN26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1895386.6589329557</v>
       </c>
       <c r="KO26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1933294.3921116148</v>
       </c>
       <c r="KP26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>1971960.2799538472</v>
       </c>
       <c r="KQ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2011399.4855529242</v>
       </c>
       <c r="KR26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2051627.4752639828</v>
       </c>
       <c r="KS26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2092660.0247692624</v>
       </c>
       <c r="KT26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2134513.2252646475</v>
       </c>
       <c r="KU26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2177203.4897699407</v>
       </c>
       <c r="KV26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2220747.5595653397</v>
       </c>
       <c r="KW26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2265162.5107566467</v>
       </c>
       <c r="KX26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2310465.7609717799</v>
       </c>
       <c r="KY26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2356675.0761912158</v>
       </c>
       <c r="KZ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2403808.5777150402</v>
       </c>
       <c r="LA26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2451884.7492693411</v>
       </c>
       <c r="LB26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2500922.444254728</v>
       </c>
       <c r="LC26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2550940.8931398224</v>
       </c>
       <c r="LD26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2601959.711002619</v>
       </c>
       <c r="LE26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2653998.9052226716</v>
       </c>
       <c r="LF26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2707078.8833271251</v>
       </c>
       <c r="LG26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2761220.4609936676</v>
       </c>
       <c r="LH26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2816444.8702135412</v>
       </c>
       <c r="LI26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2872773.7676178119</v>
       </c>
       <c r="LJ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2930229.2429701681</v>
       </c>
       <c r="LK26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>2988833.8278295714</v>
       </c>
       <c r="LL26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3048610.5043861629</v>
       </c>
       <c r="LM26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3109582.7144738859</v>
       </c>
       <c r="LN26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3171774.3687633639</v>
       </c>
       <c r="LO26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3235209.8561386312</v>
       </c>
       <c r="LP26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3299914.0532614039</v>
       </c>
       <c r="LQ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3365912.3343266319</v>
       </c>
       <c r="LR26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3433230.5810131645</v>
       </c>
       <c r="LS26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3501895.1926334277</v>
       </c>
       <c r="LT26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3571933.0964860963</v>
       </c>
       <c r="LU26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3643371.7584158182</v>
       </c>
       <c r="LV26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3716239.1935841348</v>
       </c>
       <c r="LW26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3790563.9774558176</v>
       </c>
       <c r="LX26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3866375.2570049339</v>
       </c>
       <c r="LY26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>3943702.7621450326</v>
       </c>
       <c r="LZ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4022576.8173879334</v>
       </c>
       <c r="MA26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4103028.3537356923</v>
       </c>
       <c r="MB26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4185088.9208104061</v>
       </c>
       <c r="MC26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4268790.6992266141</v>
       </c>
       <c r="MD26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4354166.513211146</v>
       </c>
       <c r="ME26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4441249.8434753688</v>
       </c>
       <c r="MF26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4530074.8403448761</v>
       </c>
       <c r="MG26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4620676.3371517733</v>
       </c>
       <c r="MH26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4713089.863894809</v>
       </c>
       <c r="MI26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4807351.6611727057</v>
       </c>
       <c r="MJ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>4903498.6943961596</v>
       </c>
       <c r="MK26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5001568.6682840828</v>
       </c>
       <c r="ML26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5101600.0416497644</v>
       </c>
       <c r="MM26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5203632.0424827598</v>
       </c>
       <c r="MN26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5307704.6833324153</v>
       </c>
       <c r="MO26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5413858.7769990638</v>
       </c>
       <c r="MP26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5522135.9525390454</v>
       </c>
       <c r="MQ26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5632578.6715898262</v>
       </c>
       <c r="MR26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5745230.2450216226</v>
       </c>
       <c r="MS26" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>5860134.8499220554</v>
       </c>
       <c r="MT26" s="8">
-        <f t="shared" ref="MT26:PE26" si="41">MS26*(1+$AN$15)</f>
+        <f t="shared" ref="MT26:PE26" si="42">MS26*(1+$AN$15)</f>
         <v>5977337.546920497</v>
       </c>
       <c r="MU26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6096884.2978589069</v>
       </c>
       <c r="MV26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6218821.9838160854</v>
       </c>
       <c r="MW26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6343198.4234924074</v>
       </c>
       <c r="MX26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6470062.3919622554</v>
       </c>
       <c r="MY26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6599463.6398015004</v>
       </c>
       <c r="MZ26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6731452.9125975305</v>
       </c>
       <c r="NA26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>6866081.9708494814</v>
       </c>
       <c r="NB26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7003403.6102664713</v>
       </c>
       <c r="NC26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7143471.6824718006</v>
       </c>
       <c r="ND26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7286341.1161212372</v>
       </c>
       <c r="NE26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7432067.9384436617</v>
       </c>
       <c r="NF26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7580709.2972125346</v>
       </c>
       <c r="NG26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7732323.4831567854</v>
       </c>
       <c r="NH26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>7886969.9528199211</v>
       </c>
       <c r="NI26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>8044709.3518763194</v>
       </c>
       <c r="NJ26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>8205603.538913846</v>
       </c>
       <c r="NK26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>8369715.6096921228</v>
       </c>
       <c r="NL26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>8537109.9218859654</v>
       </c>
       <c r="NM26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>8707852.1203236841</v>
       </c>
       <c r="NN26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>8882009.1627301574</v>
       </c>
       <c r="NO26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>9059649.3459847607</v>
       </c>
       <c r="NP26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>9240842.3329044562</v>
       </c>
       <c r="NQ26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>9425659.1795625463</v>
       </c>
       <c r="NR26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>9614172.3631537966</v>
       </c>
       <c r="NS26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>9806455.8104168735</v>
       </c>
       <c r="NT26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>10002584.926625211</v>
       </c>
       <c r="NU26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>10202636.625157716</v>
       </c>
       <c r="NV26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>10406689.357660871</v>
       </c>
       <c r="NW26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>10614823.144814089</v>
       </c>
       <c r="NX26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>10827119.607710371</v>
       </c>
       <c r="NY26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>11043661.999864578</v>
       </c>
       <c r="NZ26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>11264535.23986187</v>
       </c>
       <c r="OA26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>11489825.944659108</v>
       </c>
       <c r="OB26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>11719622.463552291</v>
       </c>
       <c r="OC26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>11954014.912823336</v>
       </c>
       <c r="OD26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>12193095.211079802</v>
       </c>
       <c r="OE26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>12436957.115301399</v>
       </c>
       <c r="OF26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>12685696.257607426</v>
       </c>
       <c r="OG26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>12939410.182759576</v>
       </c>
       <c r="OH26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>13198198.386414768</v>
       </c>
       <c r="OI26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>13462162.354143064</v>
       </c>
       <c r="OJ26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>13731405.601225926</v>
       </c>
       <c r="OK26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>14006033.713250445</v>
       </c>
       <c r="OL26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>14286154.387515454</v>
       </c>
       <c r="OM26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>14571877.475265764</v>
       </c>
       <c r="ON26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>14863315.024771079</v>
       </c>
       <c r="OO26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>15160581.325266501</v>
       </c>
       <c r="OP26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>15463792.951771831</v>
       </c>
       <c r="OQ26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>15773068.810807267</v>
       </c>
       <c r="OR26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>16088530.187023412</v>
       </c>
       <c r="OS26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>16410300.790763881</v>
       </c>
       <c r="OT26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>16738506.80657916</v>
       </c>
       <c r="OU26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>17073276.942710742</v>
       </c>
       <c r="OV26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>17414742.481564958</v>
       </c>
       <c r="OW26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>17763037.331196256</v>
       </c>
       <c r="OX26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>18118298.077820182</v>
       </c>
       <c r="OY26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>18480664.039376587</v>
       </c>
       <c r="OZ26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>18850277.320164118</v>
       </c>
       <c r="PA26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>19227282.866567399</v>
       </c>
       <c r="PB26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>19611828.523898747</v>
       </c>
       <c r="PC26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>20004065.09437672</v>
       </c>
       <c r="PD26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>20404146.396264255</v>
       </c>
       <c r="PE26" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>20812229.32418954</v>
       </c>
       <c r="PF26" s="8">
-        <f t="shared" ref="PF26:RQ26" si="42">PE26*(1+$AN$15)</f>
+        <f t="shared" ref="PF26:RQ26" si="43">PE26*(1+$AN$15)</f>
         <v>21228473.910673331</v>
       </c>
       <c r="PG26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>21653043.388886798</v>
       </c>
       <c r="PH26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>22086104.256664533</v>
       </c>
       <c r="PI26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>22527826.341797825</v>
       </c>
       <c r="PJ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>22978382.868633781</v>
       </c>
       <c r="PK26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>23437950.526006456</v>
       </c>
       <c r="PL26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>23906709.536526587</v>
       </c>
       <c r="PM26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>24384843.727257118</v>
       </c>
       <c r="PN26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>24872540.60180226</v>
       </c>
       <c r="PO26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>25369991.413838305</v>
       </c>
       <c r="PP26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>25877391.242115073</v>
       </c>
       <c r="PQ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>26394939.066957373</v>
       </c>
       <c r="PR26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>26922837.848296519</v>
       </c>
       <c r="PS26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>27461294.605262451</v>
       </c>
       <c r="PT26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>28010520.497367699</v>
       </c>
       <c r="PU26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>28570730.907315053</v>
       </c>
       <c r="PV26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>29142145.525461353</v>
       </c>
       <c r="PW26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>29724988.435970582</v>
       </c>
       <c r="PX26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>30319488.204689994</v>
       </c>
       <c r="PY26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>30925877.968783796</v>
       </c>
       <c r="PZ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>31544395.528159473</v>
       </c>
       <c r="QA26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>32175283.438722663</v>
       </c>
       <c r="QB26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>32818789.107497115</v>
       </c>
       <c r="QC26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>33475164.889647059</v>
       </c>
       <c r="QD26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>34144668.18744</v>
       </c>
       <c r="QE26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>34827561.551188804</v>
       </c>
       <c r="QF26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>35524112.782212578</v>
       </c>
       <c r="QG26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>36234595.037856832</v>
       </c>
       <c r="QH26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>36959286.938613966</v>
       </c>
       <c r="QI26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>37698472.677386247</v>
       </c>
       <c r="QJ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>38452442.13093397</v>
       </c>
       <c r="QK26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>39221490.973552652</v>
       </c>
       <c r="QL26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>40005920.793023705</v>
       </c>
       <c r="QM26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>40806039.20888418</v>
       </c>
       <c r="QN26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>41622159.993061863</v>
       </c>
       <c r="QO26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>42454603.192923099</v>
       </c>
       <c r="QP26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>43303695.256781563</v>
       </c>
       <c r="QQ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>44169769.161917195</v>
       </c>
       <c r="QR26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>45053164.54515554</v>
       </c>
       <c r="QS26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>45954227.836058654</v>
       </c>
       <c r="QT26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>46873312.392779827</v>
       </c>
       <c r="QU26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>47810778.640635423</v>
       </c>
       <c r="QV26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>48766994.21344813</v>
       </c>
       <c r="QW26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>49742334.097717091</v>
       </c>
       <c r="QX26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>50737180.779671431</v>
       </c>
       <c r="QY26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>51751924.395264857</v>
       </c>
       <c r="QZ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>52786962.883170158</v>
       </c>
       <c r="RA26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>53842702.140833564</v>
       </c>
       <c r="RB26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>54919556.183650233</v>
       </c>
       <c r="RC26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>56017947.30732324</v>
       </c>
       <c r="RD26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>57138306.253469706</v>
       </c>
       <c r="RE26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>58281072.3785391</v>
       </c>
       <c r="RF26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>59446693.826109886</v>
       </c>
       <c r="RG26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>60635627.702632084</v>
       </c>
       <c r="RH26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>61848340.256684728</v>
       </c>
       <c r="RI26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>63085307.061818421</v>
       </c>
       <c r="RJ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>64347013.203054793</v>
       </c>
       <c r="RK26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>65633953.467115887</v>
       </c>
       <c r="RL26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>66946632.536458202</v>
       </c>
       <c r="RM26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>68285565.187187374</v>
       </c>
       <c r="RN26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>69651276.490931123</v>
       </c>
       <c r="RO26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>71044302.020749748</v>
       </c>
       <c r="RP26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>72465188.061164737</v>
       </c>
       <c r="RQ26" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>73914491.822388038</v>
       </c>
       <c r="RR26" s="8">
-        <f t="shared" ref="RR26:UC26" si="43">RQ26*(1+$AN$15)</f>
+        <f t="shared" ref="RR26:UC26" si="44">RQ26*(1+$AN$15)</f>
         <v>75392781.658835799</v>
       </c>
       <c r="RS26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>76900637.292012513</v>
       </c>
       <c r="RT26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>78438650.037852764</v>
       </c>
       <c r="RU26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>80007423.038609818</v>
       </c>
       <c r="RV26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>81607571.499382019</v>
       </c>
       <c r="RW26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>83239722.929369658</v>
       </c>
       <c r="RX26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>84904517.387957051</v>
       </c>
       <c r="RY26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>86602607.735716194</v>
       </c>
       <c r="RZ26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>88334659.890430525</v>
       </c>
       <c r="SA26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>90101353.088239133</v>
       </c>
       <c r="SB26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>91903380.150003925</v>
       </c>
       <c r="SC26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>93741447.753004</v>
       </c>
       <c r="SD26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>95616276.708064079</v>
       </c>
       <c r="SE26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>97528602.242225364</v>
       </c>
       <c r="SF26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>99479174.287069872</v>
       </c>
       <c r="SG26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>101468757.77281126</v>
       </c>
       <c r="SH26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>103498132.92826749</v>
       </c>
       <c r="SI26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>105568095.58683285</v>
       </c>
       <c r="SJ26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>107679457.4985695</v>
       </c>
       <c r="SK26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>109833046.6485409</v>
       </c>
       <c r="SL26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>112029707.58151172</v>
       </c>
       <c r="SM26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>114270301.73314196</v>
       </c>
       <c r="SN26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>116555707.7678048</v>
       </c>
       <c r="SO26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>118886821.9231609</v>
       </c>
       <c r="SP26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>121264558.36162412</v>
       </c>
       <c r="SQ26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>123689849.52885661</v>
       </c>
       <c r="SR26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>126163646.51943374</v>
       </c>
       <c r="SS26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>128686919.44982241</v>
       </c>
       <c r="ST26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>131260657.83881886</v>
       </c>
       <c r="SU26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>133885870.99559525</v>
       </c>
       <c r="SV26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>136563588.41550717</v>
       </c>
       <c r="SW26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>139294860.18381733</v>
       </c>
       <c r="SX26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>142080757.38749367</v>
       </c>
       <c r="SY26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>144922372.53524354</v>
       </c>
       <c r="SZ26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>147820819.98594841</v>
       </c>
       <c r="TA26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>150777236.38566738</v>
       </c>
       <c r="TB26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>153792781.11338073</v>
       </c>
       <c r="TC26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>156868636.73564833</v>
       </c>
       <c r="TD26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>160006009.47036129</v>
       </c>
       <c r="TE26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>163206129.65976852</v>
       </c>
       <c r="TF26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>166470252.2529639</v>
       </c>
       <c r="TG26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>169799657.29802319</v>
       </c>
       <c r="TH26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>173195650.44398367</v>
       </c>
       <c r="TI26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>176659563.45286337</v>
       </c>
       <c r="TJ26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>180192754.72192064</v>
       </c>
       <c r="TK26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>183796609.81635904</v>
       </c>
       <c r="TL26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>187472542.01268622</v>
       </c>
       <c r="TM26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>191221992.85293996</v>
       </c>
       <c r="TN26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>195046432.70999876</v>
       </c>
       <c r="TO26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>198947361.36419874</v>
       </c>
       <c r="TP26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>202926308.59148273</v>
       </c>
       <c r="TQ26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>206984834.7633124</v>
       </c>
       <c r="TR26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>211124531.45857865</v>
       </c>
       <c r="TS26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>215347022.08775023</v>
       </c>
       <c r="TT26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>219653962.52950522</v>
       </c>
       <c r="TU26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>224047041.78009534</v>
       </c>
       <c r="TV26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>228527982.61569723</v>
       </c>
       <c r="TW26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>233098542.26801118</v>
       </c>
       <c r="TX26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>237760513.1133714</v>
       </c>
       <c r="TY26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>242515723.37563884</v>
       </c>
       <c r="TZ26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>247366037.84315163</v>
       </c>
       <c r="UA26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>252313358.60001466</v>
       </c>
       <c r="UB26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>257359625.77201495</v>
       </c>
       <c r="UC26" s="8">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>262506818.28745526</v>
       </c>
       <c r="UD26" s="8">
-        <f t="shared" ref="UD26:VG26" si="44">UC26*(1+$AN$15)</f>
+        <f t="shared" ref="UD26:VG26" si="45">UC26*(1+$AN$15)</f>
         <v>267756954.65320438</v>
       </c>
       <c r="UE26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>273112093.74626845</v>
       </c>
       <c r="UF26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>278574335.62119383</v>
       </c>
       <c r="UG26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>284145822.33361769</v>
       </c>
       <c r="UH26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>289828738.78029007</v>
       </c>
       <c r="UI26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>295625313.55589586</v>
       </c>
       <c r="UJ26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>301537819.82701379</v>
       </c>
       <c r="UK26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>307568576.22355407</v>
       </c>
       <c r="UL26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>313719947.74802518</v>
       </c>
       <c r="UM26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>319994346.7029857</v>
       </c>
       <c r="UN26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>326394233.63704544</v>
       </c>
       <c r="UO26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>332922118.30978638</v>
       </c>
       <c r="UP26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>339580560.67598212</v>
       </c>
       <c r="UQ26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>346372171.88950175</v>
       </c>
       <c r="UR26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>353299615.32729179</v>
       </c>
       <c r="US26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>360365607.63383764</v>
       </c>
       <c r="UT26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>367572919.7865144</v>
       </c>
       <c r="UU26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>374924378.18224472</v>
       </c>
       <c r="UV26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>382422865.7458896</v>
       </c>
       <c r="UW26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>390071323.06080741</v>
       </c>
       <c r="UX26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>397872749.52202356</v>
       </c>
       <c r="UY26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>405830204.51246405</v>
       </c>
       <c r="UZ26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>413946808.60271335</v>
       </c>
       <c r="VA26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>422225744.77476764</v>
       </c>
       <c r="VB26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>430670259.67026299</v>
       </c>
       <c r="VC26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>439283664.86366826</v>
       </c>
       <c r="VD26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>448069338.16094166</v>
       </c>
       <c r="VE26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>457030724.92416048</v>
       </c>
       <c r="VF26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>466171339.42264372</v>
       </c>
       <c r="VG26" s="8">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>475494766.21109658</v>
       </c>
     </row>
@@ -6185,75 +6185,75 @@
         <v>65</v>
       </c>
       <c r="G28" s="13">
-        <f>(G6-C6)/C6</f>
+        <f t="shared" ref="G28:X28" si="46">(G6-C6)/C6</f>
         <v>5.358088925317462E-2</v>
       </c>
       <c r="H28" s="13">
-        <f>(H6-D6)/D6</f>
+        <f t="shared" si="46"/>
         <v>2.9877648801878283</v>
       </c>
       <c r="I28" s="13">
-        <f>(I6-E6)/E6</f>
+        <f t="shared" si="46"/>
         <v>0.66682584250829335</v>
       </c>
       <c r="J28" s="13">
-        <f>(J6-F6)/F6</f>
+        <f t="shared" si="46"/>
         <v>0.78314929986593163</v>
       </c>
       <c r="K28" s="13">
-        <f>(K6-G6)/G6</f>
+        <f t="shared" si="46"/>
         <v>0.70136289427873033</v>
       </c>
       <c r="L28" s="13">
-        <f>(L6-H6)/H6</f>
+        <f t="shared" si="46"/>
         <v>0.57602996254681649</v>
       </c>
       <c r="M28" s="13">
-        <f>(M6-I6)/I6</f>
+        <f t="shared" si="46"/>
         <v>0.28897772088716006</v>
       </c>
       <c r="N28" s="13">
-        <f>(N6-J6)/J6</f>
+        <f t="shared" si="46"/>
         <v>0.24135554459090097</v>
       </c>
       <c r="O28" s="13">
-        <f>(O6-K6)/K6</f>
+        <f t="shared" si="46"/>
         <v>0.2047713717693837</v>
       </c>
       <c r="P28" s="13">
-        <f>(P6-L6)/L6</f>
+        <f t="shared" si="46"/>
         <v>0.1806083650190114</v>
       </c>
       <c r="Q28" s="13">
-        <f>(Q6-M6)/M6</f>
+        <f t="shared" si="46"/>
         <v>0.17787794729542303</v>
       </c>
       <c r="R28" s="13">
-        <f>(R6-N6)/N6</f>
+        <f t="shared" si="46"/>
         <v>0.16614090431125131</v>
       </c>
       <c r="S28" s="13">
-        <f>(S6-O6)/O6</f>
+        <f t="shared" si="46"/>
         <v>0.17821782178217821</v>
       </c>
       <c r="T28" s="13">
-        <f>(T6-P6)/P6</f>
+        <f t="shared" si="46"/>
         <v>0.10628019323671498</v>
       </c>
       <c r="U28" s="13">
-        <f>(U6-Q6)/Q6</f>
+        <f t="shared" si="46"/>
         <v>9.8616426258463355E-2</v>
       </c>
       <c r="V28" s="13">
-        <f>(V6-R6)/R6</f>
+        <f t="shared" si="46"/>
         <v>0.11812443642921551</v>
       </c>
       <c r="W28" s="26">
-        <f>(W6-S6)/S6</f>
+        <f t="shared" si="46"/>
         <v>6.069094304388422E-2</v>
       </c>
       <c r="X28" s="26">
-        <f>(X6-T6)/T6</f>
+        <f t="shared" si="46"/>
         <v>0.12663755458515283</v>
       </c>
       <c r="AA28" s="13"/>
@@ -6279,75 +6279,75 @@
         <v>66</v>
       </c>
       <c r="G29" s="6">
-        <f>(G19-C19)/C19</f>
+        <f t="shared" ref="G29:X29" si="47">(G19-C19)/C19</f>
         <v>2.4415554674769897</v>
       </c>
       <c r="H29" s="6">
-        <f>(H19-D19)/D19</f>
+        <f t="shared" si="47"/>
         <v>-0.88211880720237379</v>
       </c>
       <c r="I29" s="6">
-        <f>(I19-E19)/E19</f>
+        <f t="shared" si="47"/>
         <v>2.7895270208859726</v>
       </c>
       <c r="J29" s="6">
-        <f>(J19-F19)/F19</f>
+        <f t="shared" si="47"/>
         <v>-1.0140182841369179</v>
       </c>
       <c r="K29" s="6">
-        <f>(K19-G19)/G19</f>
+        <f t="shared" si="47"/>
         <v>-0.98379131402111053</v>
       </c>
       <c r="L29" s="6">
-        <f>(L19-H19)/H19</f>
+        <f t="shared" si="47"/>
         <v>-6.5857688169665849</v>
       </c>
       <c r="M29" s="6">
-        <f>(M19-I19)/I19</f>
+        <f t="shared" si="47"/>
         <v>0.45582226976362689</v>
       </c>
       <c r="N29" s="6">
-        <f>(N19-J19)/J19</f>
+        <f t="shared" si="47"/>
         <v>4.8531036127777476</v>
       </c>
       <c r="O29" s="6">
-        <f>(O19-K19)/K19</f>
+        <f t="shared" si="47"/>
         <v>-7.1578947368421053</v>
       </c>
       <c r="P29" s="6">
-        <f>(P19-L19)/L19</f>
+        <f t="shared" si="47"/>
         <v>0.71503957783641159</v>
       </c>
       <c r="Q29" s="6">
-        <f>(Q19-M19)/M19</f>
+        <f t="shared" si="47"/>
         <v>2.6029654036243821</v>
       </c>
       <c r="R29" s="6">
-        <f>(R19-N19)/N19</f>
+        <f t="shared" si="47"/>
         <v>-2.0940438871473352</v>
       </c>
       <c r="S29" s="6">
-        <f>(S19-O19)/O19</f>
+        <f t="shared" si="47"/>
         <v>1.2564102564102564</v>
       </c>
       <c r="T29" s="6">
-        <f>(T19-P19)/P19</f>
+        <f t="shared" si="47"/>
         <v>-0.14615384615384616</v>
       </c>
       <c r="U29" s="6">
-        <f>(U19-Q19)/Q19</f>
+        <f t="shared" si="47"/>
         <v>-0.68724279835390945</v>
       </c>
       <c r="V29" s="6">
-        <f>(V19-R19)/R19</f>
+        <f t="shared" si="47"/>
         <v>-2.3209169054441259</v>
       </c>
       <c r="W29" s="27">
-        <f>(W19-S19)/S19</f>
+        <f t="shared" si="47"/>
         <v>-0.41666666666666669</v>
       </c>
       <c r="X29" s="27">
-        <f>(X19-T19)/T19</f>
+        <f t="shared" si="47"/>
         <v>0.15675675675675677</v>
       </c>
       <c r="AA29" s="6"/>
@@ -6377,71 +6377,71 @@
         <v>2.0547874179052887</v>
       </c>
       <c r="H30" s="13">
-        <f t="shared" ref="H30:X30" si="45">(H26-D26)/ABS(D26)</f>
+        <f t="shared" ref="H30:X30" si="48">(H26-D26)/ABS(D26)</f>
         <v>3.9737742303306733</v>
       </c>
       <c r="I30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.57907469005140599</v>
       </c>
       <c r="J30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>2.3856880733944954</v>
       </c>
       <c r="K30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.95969195477633962</v>
       </c>
       <c r="L30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>1.6104294478527636E-2</v>
       </c>
       <c r="M30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.83646112600536215</v>
       </c>
       <c r="N30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.20497881355932196</v>
       </c>
       <c r="O30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.32190635451505017</v>
       </c>
       <c r="P30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.13207547169811321</v>
       </c>
       <c r="Q30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.36600625651720542</v>
       </c>
       <c r="R30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>-0.89890109890109893</v>
       </c>
       <c r="S30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.20746363061353573</v>
       </c>
       <c r="T30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0.15888888888888889</v>
       </c>
       <c r="U30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>-0.18015267175572519</v>
       </c>
       <c r="V30" s="13">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>8.9565217391304355</v>
       </c>
       <c r="W30" s="26">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>-6.7050811943425881E-2</v>
       </c>
       <c r="X30" s="26">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>-8.7248322147651006E-2</v>
       </c>
       <c r="AA30" s="13"/>
@@ -6450,15 +6450,15 @@
         <v>3.9259731971920862</v>
       </c>
       <c r="AC30" s="13">
-        <f t="shared" ref="AC30:AE30" si="46">(AC26-AB26)/ABS(AB26)</f>
+        <f t="shared" ref="AC30:AE30" si="49">(AC26-AB26)/ABS(AB26)</f>
         <v>0.48527808069792833</v>
       </c>
       <c r="AD30" s="13">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0.12687224669603525</v>
       </c>
       <c r="AE30" s="13">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>0.16862131873859787</v>
       </c>
     </row>
@@ -6488,92 +6488,92 @@
         <v>70</v>
       </c>
       <c r="G32" s="6">
-        <f>(G3-C3)/C3</f>
+        <f t="shared" ref="G32:P34" si="50">(G3-C3)/C3</f>
         <v>0.12784588441331005</v>
       </c>
       <c r="H32" s="6">
-        <f>(H3-D3)/D3</f>
+        <f t="shared" si="50"/>
         <v>1.9678571428571427</v>
       </c>
       <c r="I32" s="6">
-        <f>(I3-E3)/E3</f>
+        <f t="shared" si="50"/>
         <v>0.2928802588996765</v>
       </c>
       <c r="J32" s="6">
-        <f>(J3-F3)/F3</f>
+        <f t="shared" si="50"/>
         <v>0.58531317494600454</v>
       </c>
       <c r="K32" s="6">
-        <f>(K3-G3)/G3</f>
+        <f t="shared" si="50"/>
         <v>0.58540372670807428</v>
       </c>
       <c r="L32" s="6">
-        <f>(L3-H3)/H3</f>
+        <f t="shared" si="50"/>
         <v>0.24789410348977148</v>
       </c>
       <c r="M32" s="6">
-        <f>(M3-I3)/I3</f>
+        <f t="shared" si="50"/>
         <v>0.24780976220275339</v>
       </c>
       <c r="N32" s="6">
-        <f>(N3-J3)/J3</f>
+        <f t="shared" si="50"/>
         <v>0.20163487738419614</v>
       </c>
       <c r="O32" s="6">
-        <f>(O3-K3)/K3</f>
+        <f t="shared" si="50"/>
         <v>0.1860920666013712</v>
       </c>
       <c r="P32" s="6">
-        <f>(P3-L3)/L3</f>
+        <f t="shared" si="50"/>
         <v>0.10993249758919953</v>
       </c>
       <c r="Q32" s="6">
-        <f>(Q3-M3)/M3</f>
+        <f t="shared" ref="Q32:Z34" si="51">(Q3-M3)/M3</f>
         <v>0.13540621865596791</v>
       </c>
       <c r="R32" s="6">
-        <f>(R3-N3)/N3</f>
+        <f t="shared" si="51"/>
         <v>0.12018140589569154</v>
       </c>
       <c r="S32" s="6">
-        <f>(S3-O3)/O3</f>
+        <f t="shared" si="51"/>
         <v>9.4962840627580522E-2</v>
       </c>
       <c r="T32" s="6">
-        <f>(T3-P3)/P3</f>
+        <f t="shared" si="51"/>
         <v>8.6880973066898348E-2</v>
       </c>
       <c r="U32" s="6">
-        <f>(U3-Q3)/Q3</f>
+        <f t="shared" si="51"/>
         <v>0.10512367491166071</v>
       </c>
       <c r="V32" s="6">
-        <f>(V3-R3)/R3</f>
+        <f t="shared" si="51"/>
         <v>0.24291497975708504</v>
       </c>
       <c r="W32" s="27">
-        <f>(W3-S3)/S3</f>
+        <f t="shared" si="51"/>
         <v>-0.16289592760180993</v>
       </c>
       <c r="X32" s="27">
-        <f>(X3-T3)/T3</f>
+        <f t="shared" si="51"/>
         <v>7.4340527577937743E-2</v>
       </c>
       <c r="AA32" s="6"/>
       <c r="AB32" s="6">
-        <f>(AB3-AA3)/AA3</f>
+        <f t="shared" ref="AB32:AE34" si="52">(AB3-AA3)/AA3</f>
         <v>0.55693581780538315</v>
       </c>
       <c r="AC32" s="6">
-        <f>(AC3-AB3)/AB3</f>
+        <f t="shared" si="52"/>
         <v>0.30884308510638286</v>
       </c>
       <c r="AD32" s="6">
-        <f>(AD3-AC3)/AC3</f>
+        <f t="shared" si="52"/>
         <v>0.13843027686055373</v>
       </c>
       <c r="AE32" s="6">
-        <f>(AE3-AD3)/AD3</f>
+        <f t="shared" si="52"/>
         <v>0.12806782686300755</v>
       </c>
     </row>
@@ -6582,92 +6582,92 @@
         <v>71</v>
       </c>
       <c r="G33" s="15">
-        <f>(G4-C4)/C4</f>
+        <f t="shared" si="50"/>
         <v>0.52069169376293234</v>
       </c>
       <c r="H33" s="15">
-        <f>(H4-D4)/D4</f>
+        <f t="shared" si="50"/>
         <v>3.1875</v>
       </c>
       <c r="I33" s="15">
-        <f>(I4-E4)/E4</f>
+        <f t="shared" si="50"/>
         <v>0.48749999999999999</v>
       </c>
       <c r="J33" s="15">
-        <f>(J4-F4)/F4</f>
+        <f t="shared" si="50"/>
         <v>0.91067796610169494</v>
       </c>
       <c r="K33" s="15">
-        <f>(K4-G4)/G4</f>
+        <f t="shared" si="50"/>
         <v>0.67168821071046747</v>
       </c>
       <c r="L33" s="15">
-        <f>(L4-H4)/H4</f>
+        <f t="shared" si="50"/>
         <v>0.26119402985074625</v>
       </c>
       <c r="M33" s="15">
-        <f>(M4-I4)/I4</f>
+        <f t="shared" si="50"/>
         <v>0.31092436974789917</v>
       </c>
       <c r="N33" s="15">
-        <f>(N4-J4)/J4</f>
+        <f t="shared" si="50"/>
         <v>0.19755167213696442</v>
       </c>
       <c r="O33" s="15">
-        <f>(O4-K4)/K4</f>
+        <f t="shared" si="50"/>
         <v>0.18604651162790697</v>
       </c>
       <c r="P33" s="15">
-        <f>(P4-L4)/L4</f>
+        <f t="shared" si="50"/>
         <v>0.13017751479289941</v>
       </c>
       <c r="Q33" s="15">
-        <f>(Q4-M4)/M4</f>
+        <f t="shared" si="51"/>
         <v>0.17307692307692307</v>
       </c>
       <c r="R33" s="15">
-        <f>(R4-N4)/N4</f>
+        <f t="shared" si="51"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="S33" s="15">
-        <f>(S4-O4)/O4</f>
+        <f t="shared" si="51"/>
         <v>0.12254901960784313</v>
       </c>
       <c r="T33" s="15">
-        <f>(T4-P4)/P4</f>
+        <f t="shared" si="51"/>
         <v>0.1099476439790576</v>
       </c>
       <c r="U33" s="15">
-        <f>(U4-Q4)/Q4</f>
+        <f t="shared" si="51"/>
         <v>0.15846994535519127</v>
       </c>
       <c r="V33" s="15">
-        <f>(V4-R4)/R4</f>
+        <f t="shared" si="51"/>
         <v>0.29677419354838708</v>
       </c>
       <c r="W33" s="28">
-        <f>(W4-S4)/S4</f>
+        <f t="shared" si="51"/>
         <v>-0.23144104803493451</v>
       </c>
       <c r="X33" s="28">
-        <f>(X4-T4)/T4</f>
+        <f t="shared" si="51"/>
         <v>0.10849056603773585</v>
       </c>
       <c r="AA33" s="15"/>
       <c r="AB33" s="15">
-        <f>(AB4-AA4)/AA4</f>
+        <f t="shared" si="52"/>
         <v>0.96354646777842956</v>
       </c>
       <c r="AC33" s="15">
-        <f>(AC4-AB4)/AB4</f>
+        <f t="shared" si="52"/>
         <v>0.34864068968460588</v>
       </c>
       <c r="AD33" s="15">
-        <f>(AD4-AC4)/AC4</f>
+        <f t="shared" si="52"/>
         <v>0.15981012658227847</v>
       </c>
       <c r="AE33" s="15">
-        <f>(AE4-AD4)/AD4</f>
+        <f t="shared" si="52"/>
         <v>0.165075034106412</v>
       </c>
     </row>
@@ -6676,92 +6676,92 @@
         <v>72</v>
       </c>
       <c r="G34" s="6">
-        <f>(G5-C5)/C5</f>
+        <f t="shared" si="50"/>
         <v>0.34831515083638848</v>
       </c>
       <c r="H34" s="6">
-        <f>(H5-D5)/D5</f>
+        <f t="shared" si="50"/>
         <v>0.41095066185318885</v>
       </c>
       <c r="I34" s="6">
-        <f>(I5-E5)/E5</f>
+        <f t="shared" si="50"/>
         <v>0.15053191489361675</v>
       </c>
       <c r="J34" s="6">
-        <f>(J5-F5)/F5</f>
+        <f t="shared" si="50"/>
         <v>0.20523691867177743</v>
       </c>
       <c r="K34" s="6">
-        <f>(K5-G5)/G5</f>
+        <f t="shared" si="50"/>
         <v>5.4424297451068936E-2</v>
       </c>
       <c r="L34" s="6">
-        <f>(L5-H5)/H5</f>
+        <f t="shared" si="50"/>
         <v>1.0657896630636534E-2</v>
       </c>
       <c r="M34" s="6">
-        <f>(M5-I5)/I5</f>
+        <f t="shared" si="50"/>
         <v>5.058031236566856E-2</v>
       </c>
       <c r="N34" s="6">
-        <f>(N5-J5)/J5</f>
+        <f t="shared" si="50"/>
         <v>-3.3980415549525237E-3</v>
       </c>
       <c r="O34" s="6">
-        <f>(O5-K5)/K5</f>
+        <f t="shared" si="50"/>
         <v>-3.8407620071875675E-5</v>
       </c>
       <c r="P34" s="6">
-        <f>(P5-L5)/L5</f>
+        <f t="shared" si="50"/>
         <v>1.8239863458068408E-2</v>
       </c>
       <c r="Q34" s="6">
-        <f>(Q5-M5)/M5</f>
+        <f t="shared" si="51"/>
         <v>3.3178173416689272E-2</v>
       </c>
       <c r="R34" s="6">
-        <f>(R5-N5)/N5</f>
+        <f t="shared" si="51"/>
         <v>2.4966261808367186E-2</v>
       </c>
       <c r="S34" s="6">
-        <f>(S5-O5)/O5</f>
+        <f t="shared" si="51"/>
         <v>2.5193712477449413E-2</v>
       </c>
       <c r="T34" s="6">
-        <f>(T5-P5)/P5</f>
+        <f t="shared" si="51"/>
         <v>2.1222812326055458E-2</v>
       </c>
       <c r="U34" s="6">
-        <f>(U5-Q5)/Q5</f>
+        <f t="shared" si="51"/>
         <v>4.8271765101580003E-2</v>
       </c>
       <c r="V34" s="6">
-        <f>(V5-R5)/R5</f>
+        <f t="shared" si="51"/>
         <v>4.3332983082904314E-2</v>
       </c>
       <c r="W34" s="27">
-        <f>(W5-S5)/S5</f>
+        <f t="shared" si="51"/>
         <v>-8.1883630355246054E-2</v>
       </c>
       <c r="X34" s="27">
-        <f>(X5-T5)/T5</f>
+        <f t="shared" si="51"/>
         <v>3.1786977762803224E-2</v>
       </c>
       <c r="AA34" s="6"/>
       <c r="AB34" s="6">
-        <f>(AB5-AA5)/AA5</f>
+        <f t="shared" si="52"/>
         <v>0.27341184471806901</v>
       </c>
       <c r="AC34" s="6">
-        <f>(AC5-AB5)/AB5</f>
+        <f t="shared" si="52"/>
         <v>2.794564741155459E-2</v>
       </c>
       <c r="AD34" s="6">
-        <f>(AD5-AC5)/AC5</f>
+        <f t="shared" si="52"/>
         <v>1.8688781470470681E-2</v>
       </c>
       <c r="AE34" s="6">
-        <f>(AE5-AD5)/AD5</f>
+        <f t="shared" si="52"/>
         <v>3.4256709411908226E-2</v>
       </c>
     </row>
@@ -6770,91 +6770,91 @@
         <v>49</v>
       </c>
       <c r="C36" s="6">
-        <f>C8/C6</f>
+        <f t="shared" ref="C36:X36" si="53">C8/C6</f>
         <v>0.67003789363648236</v>
       </c>
       <c r="D36" s="6">
-        <f>D8/D6</f>
+        <f t="shared" si="53"/>
         <v>0.51848709875916288</v>
       </c>
       <c r="E36" s="6">
-        <f>E8/E6</f>
+        <f t="shared" si="53"/>
         <v>0.83064907239719554</v>
       </c>
       <c r="F36" s="6">
-        <f>F8/F6</f>
+        <f t="shared" si="53"/>
         <v>0.75589923469387765</v>
       </c>
       <c r="G36" s="6">
-        <f>G8/G6</f>
+        <f t="shared" si="53"/>
         <v>0.71304017426285549</v>
       </c>
       <c r="H36" s="6">
-        <f>H8/H6</f>
+        <f t="shared" si="53"/>
         <v>0.77945543071161039</v>
       </c>
       <c r="I36" s="6">
-        <f>I8/I6</f>
+        <f t="shared" si="53"/>
         <v>0.86074213652079712</v>
       </c>
       <c r="J36" s="6">
-        <f>J8/J6</f>
+        <f t="shared" si="53"/>
         <v>0.80726290892287933</v>
       </c>
       <c r="K36" s="6">
-        <f>K8/K6</f>
+        <f t="shared" si="53"/>
         <v>0.75944333996023861</v>
       </c>
       <c r="L36" s="6">
-        <f>L8/L6</f>
+        <f t="shared" si="53"/>
         <v>0.81463878326996197</v>
       </c>
       <c r="M36" s="6">
-        <f>M8/M6</f>
+        <f t="shared" si="53"/>
         <v>0.86095700416088761</v>
       </c>
       <c r="N36" s="6">
-        <f>N8/N6</f>
+        <f t="shared" si="53"/>
         <v>0.81861198738170349</v>
       </c>
       <c r="O36" s="6">
-        <f>O8/O6</f>
+        <f t="shared" si="53"/>
         <v>0.76457645764576454</v>
       </c>
       <c r="P36" s="6">
-        <f>P8/P6</f>
+        <f t="shared" si="53"/>
         <v>0.82608695652173914</v>
       </c>
       <c r="Q36" s="6">
-        <f>Q8/Q6</f>
+        <f t="shared" si="53"/>
         <v>0.8648807771563144</v>
       </c>
       <c r="R36" s="6">
-        <f>R8/R6</f>
+        <f t="shared" si="53"/>
         <v>0.82687105500450853</v>
       </c>
       <c r="S36" s="6">
-        <f>S8/S6</f>
+        <f t="shared" si="53"/>
         <v>0.77591036414565828</v>
       </c>
       <c r="T36" s="6">
-        <f>T8/T6</f>
+        <f t="shared" si="53"/>
         <v>0.81586608442503639</v>
       </c>
       <c r="U36" s="6">
-        <f>U8/U6</f>
+        <f t="shared" si="53"/>
         <v>0.87540192926045013</v>
       </c>
       <c r="V36" s="6">
-        <f>V8/V6</f>
+        <f t="shared" si="53"/>
         <v>0.82782258064516134</v>
       </c>
       <c r="W36" s="27">
-        <f>W8/W6</f>
+        <f t="shared" si="53"/>
         <v>0.77728873239436624</v>
       </c>
       <c r="X36" s="27">
-        <f>X8/X6</f>
+        <f t="shared" si="53"/>
         <v>0.82428940568475451</v>
       </c>
       <c r="AA36" s="6">
@@ -6883,91 +6883,91 @@
         <v>50</v>
       </c>
       <c r="C37" s="6">
-        <f>C14/C6</f>
+        <f t="shared" ref="C37:X37" si="54">C14/C6</f>
         <v>-0.38664457194445423</v>
       </c>
       <c r="D37" s="6">
-        <f>D14/D6</f>
+        <f t="shared" si="54"/>
         <v>-1.7421155764784602</v>
       </c>
       <c r="E37" s="6">
-        <f>E14/E6</f>
+        <f t="shared" si="54"/>
         <v>0.31194764927577473</v>
       </c>
       <c r="F37" s="6">
-        <f>F14/F6</f>
+        <f t="shared" si="54"/>
         <v>-3.6079481975271865</v>
       </c>
       <c r="G37" s="6">
-        <f>G14/G6</f>
+        <f t="shared" si="54"/>
         <v>-0.50392023776236372</v>
       </c>
       <c r="H37" s="6">
-        <f>H14/H6</f>
+        <f t="shared" si="54"/>
         <v>-3.8136329588015008E-2</v>
       </c>
       <c r="I37" s="6">
-        <f>I14/I6</f>
+        <f t="shared" si="54"/>
         <v>0.38078162822378514</v>
       </c>
       <c r="J37" s="6">
-        <f>J14/J6</f>
+        <f t="shared" si="54"/>
         <v>4.931940822192462E-2</v>
       </c>
       <c r="K37" s="6">
-        <f>K14/K6</f>
+        <f t="shared" si="54"/>
         <v>-3.3134526176275677E-3</v>
       </c>
       <c r="L37" s="6">
-        <f>L14/L6</f>
+        <f t="shared" si="54"/>
         <v>0.17538022813688212</v>
       </c>
       <c r="M37" s="6">
-        <f>M14/M6</f>
+        <f t="shared" si="54"/>
         <v>0.41712898751733701</v>
       </c>
       <c r="N37" s="6">
-        <f>N14/N6</f>
+        <f t="shared" si="54"/>
         <v>0.12355415352260778</v>
       </c>
       <c r="O37" s="6">
-        <f>O14/O6</f>
+        <f t="shared" si="54"/>
         <v>-2.7502750275027505E-3</v>
       </c>
       <c r="P37" s="6">
-        <f>P14/P6</f>
+        <f t="shared" si="54"/>
         <v>0.21054750402576489</v>
       </c>
       <c r="Q37" s="6">
-        <f>Q14/Q6</f>
+        <f t="shared" si="54"/>
         <v>0.44038857815719751</v>
       </c>
       <c r="R37" s="6">
-        <f>R14/R6</f>
+        <f t="shared" si="54"/>
         <v>-0.22362488728584309</v>
       </c>
       <c r="S37" s="6">
-        <f>S14/S6</f>
+        <f t="shared" si="54"/>
         <v>4.7152194211017739E-2</v>
       </c>
       <c r="T37" s="6">
-        <f>T14/T6</f>
+        <f t="shared" si="54"/>
         <v>0.18085880640465793</v>
       </c>
       <c r="U37" s="6">
-        <f>U14/U6</f>
+        <f t="shared" si="54"/>
         <v>0.40862808145766344</v>
       </c>
       <c r="V37" s="6">
-        <f>V14/V6</f>
+        <f t="shared" si="54"/>
         <v>0.17338709677419356</v>
       </c>
       <c r="W37" s="27">
-        <f>W14/W6</f>
+        <f t="shared" si="54"/>
         <v>1.6725352112676055E-2</v>
       </c>
       <c r="X37" s="27">
-        <f>X14/X6</f>
+        <f t="shared" si="54"/>
         <v>0.19767441860465115</v>
       </c>
       <c r="AA37" s="6">
@@ -6996,91 +6996,91 @@
         <v>51</v>
       </c>
       <c r="C38" s="6">
-        <f>C19/C6</f>
+        <f t="shared" ref="C38:X38" si="55">C19/C6</f>
         <v>-0.4046006913509852</v>
       </c>
       <c r="D38" s="6">
-        <f>D19/D6</f>
+        <f t="shared" si="55"/>
         <v>-1.7193330425899263</v>
       </c>
       <c r="E38" s="6">
-        <f>E19/E6</f>
+        <f t="shared" si="55"/>
         <v>0.16393274088134743</v>
       </c>
       <c r="F38" s="6">
-        <f>F19/F6</f>
+        <f t="shared" si="55"/>
         <v>-4.5246292175629383</v>
       </c>
       <c r="G38" s="6">
-        <f>G19/G6</f>
+        <f t="shared" si="55"/>
         <v>-1.3216410203216464</v>
       </c>
       <c r="H38" s="6">
-        <f>H19/H6</f>
+        <f t="shared" si="55"/>
         <v>-5.0824719101123628E-2</v>
       </c>
       <c r="I38" s="6">
-        <f>I19/I6</f>
+        <f t="shared" si="55"/>
         <v>0.37270093571558821</v>
       </c>
       <c r="J38" s="6">
-        <f>J19/J6</f>
+        <f t="shared" si="55"/>
         <v>3.5570514477260097E-2</v>
       </c>
       <c r="K38" s="6">
-        <f>K19/K6</f>
+        <f t="shared" si="55"/>
         <v>-1.2591119946984758E-2</v>
       </c>
       <c r="L38" s="6">
-        <f>L19/L6</f>
+        <f t="shared" si="55"/>
         <v>0.18013307984790874</v>
       </c>
       <c r="M38" s="6">
-        <f>M19/M6</f>
+        <f t="shared" si="55"/>
         <v>0.42094313453536752</v>
       </c>
       <c r="N38" s="6">
-        <f>N19/N6</f>
+        <f t="shared" si="55"/>
         <v>0.16771819137749738</v>
       </c>
       <c r="O38" s="6">
-        <f>O19/O6</f>
+        <f t="shared" si="55"/>
         <v>6.4356435643564358E-2</v>
       </c>
       <c r="P38" s="6">
-        <f>P19/P6</f>
+        <f t="shared" si="55"/>
         <v>0.26167471819645732</v>
       </c>
       <c r="Q38" s="6">
-        <f>Q19/Q6</f>
+        <f t="shared" si="55"/>
         <v>1.2876067118045333</v>
       </c>
       <c r="R38" s="6">
-        <f>R19/R6</f>
+        <f t="shared" si="55"/>
         <v>-0.15734896302975654</v>
       </c>
       <c r="S38" s="6">
-        <f>S19/S6</f>
+        <f t="shared" si="55"/>
         <v>0.12324929971988796</v>
       </c>
       <c r="T38" s="6">
-        <f>T19/T6</f>
+        <f t="shared" si="55"/>
         <v>0.20196506550218341</v>
       </c>
       <c r="U38" s="6">
-        <f>U19/U6</f>
+        <f t="shared" si="55"/>
         <v>0.36655948553054662</v>
       </c>
       <c r="V38" s="6">
-        <f>V19/V6</f>
+        <f t="shared" si="55"/>
         <v>0.18588709677419354</v>
       </c>
       <c r="W38" s="27">
-        <f>W19/W6</f>
+        <f t="shared" si="55"/>
         <v>6.7781690140845077E-2</v>
       </c>
       <c r="X38" s="27">
-        <f>X19/X6</f>
+        <f t="shared" si="55"/>
         <v>0.20736434108527133</v>
       </c>
       <c r="AA38" s="6">
@@ -7109,91 +7109,91 @@
         <v>76</v>
       </c>
       <c r="C39" s="13">
-        <f>C6/C4</f>
+        <f t="shared" ref="C39:X39" si="56">C6/C4</f>
         <v>0.1244206325746379</v>
       </c>
       <c r="D39" s="13">
-        <f>D6/D4</f>
+        <f t="shared" si="56"/>
         <v>0.104616875</v>
       </c>
       <c r="E39" s="13">
-        <f>E6/E4</f>
+        <f t="shared" si="56"/>
         <v>0.16779137499999999</v>
       </c>
       <c r="F39" s="13">
-        <f>F6/F4</f>
+        <f t="shared" si="56"/>
         <v>0.14563796610169491</v>
       </c>
       <c r="G39" s="13">
-        <f>G6/G4</f>
+        <f t="shared" si="56"/>
         <v>8.6202352026436002E-2</v>
       </c>
       <c r="H39" s="13">
-        <f>H6/H4</f>
+        <f t="shared" si="56"/>
         <v>9.9626865671641793E-2</v>
       </c>
       <c r="I39" s="13">
-        <f>I6/I4</f>
+        <f t="shared" si="56"/>
         <v>0.18801949579831931</v>
       </c>
       <c r="J39" s="13">
-        <f>J6/J4</f>
+        <f t="shared" si="56"/>
         <v>0.1359173245808569</v>
       </c>
       <c r="K39" s="13">
-        <f>K6/K4</f>
+        <f t="shared" si="56"/>
         <v>8.7732558139534886E-2</v>
       </c>
       <c r="L39" s="13">
-        <f>L6/L4</f>
+        <f t="shared" si="56"/>
         <v>0.12449704142011835</v>
       </c>
       <c r="M39" s="13">
-        <f>M6/M4</f>
+        <f t="shared" si="56"/>
         <v>0.18487179487179486</v>
       </c>
       <c r="N39" s="13">
-        <f>N6/N4</f>
+        <f t="shared" si="56"/>
         <v>0.1408888888888889</v>
       </c>
       <c r="O39" s="13">
-        <f>O6/O4</f>
+        <f t="shared" si="56"/>
         <v>8.9117647058823524E-2</v>
       </c>
       <c r="P39" s="13">
-        <f>P6/P4</f>
+        <f t="shared" si="56"/>
         <v>0.13005235602094239</v>
       </c>
       <c r="Q39" s="13">
-        <f>Q6/Q4</f>
+        <f t="shared" si="56"/>
         <v>0.18562841530054644</v>
       </c>
       <c r="R39" s="13">
-        <f>R6/R4</f>
+        <f t="shared" si="56"/>
         <v>0.14309677419354838</v>
       </c>
       <c r="S39" s="13">
-        <f>S6/S4</f>
+        <f t="shared" si="56"/>
         <v>9.3537117903930128E-2</v>
       </c>
       <c r="T39" s="13">
-        <f>T6/T4</f>
+        <f t="shared" si="56"/>
         <v>0.12962264150943395</v>
       </c>
       <c r="U39" s="13">
-        <f>U6/U4</f>
+        <f t="shared" si="56"/>
         <v>0.1760377358490566</v>
       </c>
       <c r="V39" s="13">
-        <f>V6/V4</f>
+        <f t="shared" si="56"/>
         <v>0.12338308457711443</v>
       </c>
       <c r="W39" s="26">
-        <f>W6/W4</f>
+        <f t="shared" si="56"/>
         <v>0.12909090909090909</v>
       </c>
       <c r="X39" s="26">
-        <f>X6/X4</f>
+        <f t="shared" si="56"/>
         <v>0.13174468085106383</v>
       </c>
       <c r="AA39" s="13">
@@ -7222,91 +7222,91 @@
         <v>52</v>
       </c>
       <c r="C41" s="1">
-        <f>C19/C21</f>
+        <f t="shared" ref="C41:X41" si="57">C19/C21</f>
         <v>-1.2974983714844057</v>
       </c>
       <c r="D41" s="1">
-        <f>D19/D21</f>
+        <f t="shared" si="57"/>
         <v>-2.18425376730913</v>
       </c>
       <c r="E41" s="1">
-        <f>E19/E21</f>
+        <f t="shared" si="57"/>
         <v>0.73545316604613531</v>
       </c>
       <c r="F41" s="1">
-        <f>F19/F21</f>
+        <f t="shared" si="57"/>
         <v>-11.244525748000754</v>
       </c>
       <c r="G41" s="1">
-        <f>G19/G21</f>
+        <f t="shared" si="57"/>
         <v>-1.950564097444089</v>
       </c>
       <c r="H41" s="1">
-        <f>H19/H21</f>
+        <f t="shared" si="57"/>
         <v>-0.11091494902237725</v>
       </c>
       <c r="I41" s="1">
-        <f>I19/I21</f>
+        <f t="shared" si="57"/>
         <v>1.2228676259246005</v>
       </c>
       <c r="J41" s="1">
-        <f>J19/J21</f>
+        <f t="shared" si="57"/>
         <v>8.0043060907980079E-2</v>
       </c>
       <c r="K41" s="1">
-        <f>K19/K21</f>
+        <f t="shared" si="57"/>
         <v>-2.9921259842519685E-2</v>
       </c>
       <c r="L41" s="1">
-        <f>L19/L21</f>
+        <f t="shared" si="57"/>
         <v>0.55409356725146197</v>
       </c>
       <c r="M41" s="1">
-        <f>M19/M21</f>
+        <f t="shared" si="57"/>
         <v>1.7774524158125915</v>
       </c>
       <c r="N41" s="1">
-        <f>N19/N21</f>
+        <f t="shared" si="57"/>
         <v>0.46911764705882353</v>
       </c>
       <c r="O41" s="1">
-        <f>O19/O21</f>
+        <f t="shared" si="57"/>
         <v>0.17462686567164179</v>
       </c>
       <c r="P41" s="1">
-        <f>P19/P21</f>
+        <f t="shared" si="57"/>
         <v>0.97744360902255634</v>
       </c>
       <c r="Q41" s="1">
-        <f>Q19/Q21</f>
+        <f t="shared" si="57"/>
         <v>6.627272727272727</v>
       </c>
       <c r="R41" s="1">
-        <f>R19/R21</f>
+        <f t="shared" si="57"/>
         <v>-0.52719033232628398</v>
       </c>
       <c r="S41" s="1">
-        <f>S19/S21</f>
+        <f t="shared" si="57"/>
         <v>0.40366972477064222</v>
       </c>
       <c r="T41" s="1">
-        <f>T19/T21</f>
+        <f t="shared" si="57"/>
         <v>0.85516178736517723</v>
       </c>
       <c r="U41" s="1">
-        <f>U19/U21</f>
+        <f t="shared" si="57"/>
         <v>2.1308411214953269</v>
       </c>
       <c r="V41" s="1">
-        <f>V19/V21</f>
+        <f t="shared" si="57"/>
         <v>0.71472868217054264</v>
       </c>
       <c r="W41" s="29">
-        <f>W19/W21</f>
+        <f t="shared" si="57"/>
         <v>0.24367088607594936</v>
       </c>
       <c r="X41" s="29">
-        <f>X19/X21</f>
+        <f t="shared" si="57"/>
         <v>1.0338164251207729</v>
       </c>
       <c r="AA41" s="1">
@@ -7524,16 +7524,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DC0004-40B4-4872-AA14-5907BAA2D76E}">
   <dimension ref="B3:H18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="18"/>
-    <col min="2" max="2" width="20.85546875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="18" customWidth="1"/>
-    <col min="4" max="16384" width="12.140625" style="18"/>
+    <col min="1" max="1" width="12.1640625" style="18"/>
+    <col min="2" max="2" width="20.83203125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="18" customWidth="1"/>
+    <col min="4" max="16384" width="12.1640625" style="18"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">

</xml_diff>